<commit_message>
cost of diversion + small updates to different values + emissions cost test table colour
</commit_message>
<xml_diff>
--- a/data/emissions_cost.xlsx
+++ b/data/emissions_cost.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oburdash\dev\repos\standard_inputs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CC4FD5-3C9A-4121-8078-2000E074258A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA4A38F-11FB-4205-BE1C-D546E0899C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="marginal" sheetId="1" r:id="rId1"/>
@@ -39,17 +39,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>class</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>Short-haul</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
@@ -62,16 +56,10 @@
     <t>Embraer 170</t>
   </si>
   <si>
-    <t>Medium-haul</t>
-  </si>
-  <si>
     <t>Airbus 320</t>
   </si>
   <si>
     <t>Boeing 737</t>
-  </si>
-  <si>
-    <t>Long-haul</t>
   </si>
   <si>
     <t>Airbus 340</t>
@@ -464,273 +452,239 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.88671875" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.88671875" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>500</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="D2">
+        <v>120</v>
+      </c>
+      <c r="E2">
+        <v>0.33</v>
+      </c>
+      <c r="F2">
+        <v>1.68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>500</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="E2">
-        <v>120</v>
-      </c>
-      <c r="F2">
-        <v>0.33</v>
-      </c>
-      <c r="G2">
-        <v>1.68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>500</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3">
+        <v>162</v>
+      </c>
+      <c r="E3">
+        <v>0.36</v>
+      </c>
+      <c r="F3">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1500</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4">
+        <v>196</v>
+      </c>
+      <c r="E4">
+        <v>0.08</v>
+      </c>
+      <c r="F4">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1500</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="E3">
-        <v>162</v>
-      </c>
-      <c r="F3">
-        <v>0.36</v>
-      </c>
-      <c r="G3">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="D5">
+        <v>219</v>
+      </c>
+      <c r="E5">
+        <v>0.13</v>
+      </c>
+      <c r="F5">
+        <v>1.87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3000</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>260</v>
+      </c>
+      <c r="E6">
+        <v>0.06</v>
+      </c>
+      <c r="F6">
+        <v>1.74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>3000</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>290</v>
+      </c>
+      <c r="E7">
+        <v>0.08</v>
+      </c>
+      <c r="F7">
+        <v>2.48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>5000</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
-        <v>1500</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D8">
+        <v>595</v>
+      </c>
+      <c r="E8">
+        <v>0.04</v>
+      </c>
+      <c r="F8">
+        <v>2.0099999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>5000</v>
+      </c>
+      <c r="B9" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="E4">
-        <v>196</v>
-      </c>
-      <c r="F4">
-        <v>0.08</v>
-      </c>
-      <c r="G4">
-        <v>1.32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="D9">
+        <v>987</v>
+      </c>
+      <c r="E9">
+        <v>0.05</v>
+      </c>
+      <c r="F9">
+        <v>2.2799999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>15000</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
-        <v>1500</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5">
-        <v>219</v>
-      </c>
-      <c r="F5">
-        <v>0.13</v>
-      </c>
-      <c r="G5">
-        <v>1.87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>3000</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D10">
+        <v>843</v>
+      </c>
+      <c r="E10">
+        <v>0.02</v>
+      </c>
+      <c r="F10">
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>15000</v>
+      </c>
+      <c r="B11" t="s">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C11" t="s">
         <v>8</v>
       </c>
-      <c r="E6">
-        <v>260</v>
-      </c>
-      <c r="F6">
-        <v>0.06</v>
-      </c>
-      <c r="G6">
-        <v>1.74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>3000</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7">
-        <v>290</v>
-      </c>
-      <c r="F7">
-        <v>0.08</v>
-      </c>
-      <c r="G7">
-        <v>2.48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>5000</v>
-      </c>
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8">
-        <v>595</v>
-      </c>
-      <c r="F8">
-        <v>0.04</v>
-      </c>
-      <c r="G8">
-        <v>2.0099999999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>5000</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9">
-        <v>987</v>
-      </c>
-      <c r="F9">
-        <v>0.05</v>
-      </c>
-      <c r="G9">
-        <v>2.2799999999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>15000</v>
-      </c>
-      <c r="C10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10">
-        <v>843</v>
-      </c>
-      <c r="F10">
+      <c r="D11">
+        <v>1397</v>
+      </c>
+      <c r="E11">
         <v>0.02</v>
       </c>
-      <c r="G10">
-        <v>2.86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>15000</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11">
-        <v>1397</v>
-      </c>
       <c r="F11">
-        <v>0.02</v>
-      </c>
-      <c r="G11">
         <v>3.22</v>
       </c>
     </row>
@@ -755,21 +709,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>71</v>
@@ -783,7 +737,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>185</v>
@@ -815,21 +769,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B2">
         <v>1.1000000000000001</v>
@@ -843,7 +797,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B3">
         <v>2.4</v>
@@ -857,7 +811,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B4">
         <v>6.6</v>
@@ -886,24 +840,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
         <v>30</v>
-      </c>
-      <c r="B1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B2">
         <v>12.9</v>

</xml_diff>